<commit_message>
Updated with different prediction method
</commit_message>
<xml_diff>
--- a/scores_2.xlsx
+++ b/scores_2.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://nd4-my.sharepoint.com/personal/sweaver4_nd_edu/Documents/Documents/Personal_projects/WCQ_Concacaf/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\simon\OneDrive - nd.edu\Documents\Personal_projects\WCQ_Concacaf\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="20" documentId="8_{9B91E494-5572-451B-B942-5B0FAD752B85}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{C3965B12-C4F8-4ABE-945A-50AE48A56FD3}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AB92F7B6-0C30-47DF-AACE-02DDC4F83BA0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="14016" xr2:uid="{26DC9B6C-8293-44D9-840D-3D50F043DF2B}"/>
+    <workbookView xWindow="28680" yWindow="-2115" windowWidth="20730" windowHeight="11160" xr2:uid="{26DC9B6C-8293-44D9-840D-3D50F043DF2B}"/>
   </bookViews>
   <sheets>
     <sheet name="scores" sheetId="1" r:id="rId1"/>
@@ -468,8 +468,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B280DDF3-1ED5-4A4B-B0D8-5D25BF88B470}">
   <dimension ref="A1:E57"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F12" sqref="F12"/>
+    <sheetView tabSelected="1" topLeftCell="A7" workbookViewId="0">
+      <selection activeCell="G20" sqref="G20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -639,8 +639,14 @@
       <c r="B10" t="s">
         <v>22</v>
       </c>
+      <c r="C10">
+        <v>1</v>
+      </c>
       <c r="D10" t="s">
         <v>21</v>
+      </c>
+      <c r="E10">
+        <v>1</v>
       </c>
     </row>
     <row r="11" spans="1:5" x14ac:dyDescent="0.3">
@@ -650,8 +656,14 @@
       <c r="B11" t="s">
         <v>19</v>
       </c>
+      <c r="C11">
+        <v>2</v>
+      </c>
       <c r="D11" t="s">
         <v>20</v>
+      </c>
+      <c r="E11">
+        <v>2</v>
       </c>
     </row>
     <row r="12" spans="1:5" x14ac:dyDescent="0.3">
@@ -661,8 +673,14 @@
       <c r="B12" t="s">
         <v>23</v>
       </c>
+      <c r="C12">
+        <v>1</v>
+      </c>
       <c r="D12" t="s">
         <v>25</v>
+      </c>
+      <c r="E12">
+        <v>2</v>
       </c>
     </row>
     <row r="13" spans="1:5" x14ac:dyDescent="0.3">
@@ -672,8 +690,14 @@
       <c r="B13" t="s">
         <v>24</v>
       </c>
+      <c r="C13">
+        <v>0</v>
+      </c>
       <c r="D13" t="s">
         <v>26</v>
+      </c>
+      <c r="E13">
+        <v>0</v>
       </c>
     </row>
     <row r="14" spans="1:5" x14ac:dyDescent="0.3">
@@ -683,8 +707,14 @@
       <c r="B14" t="s">
         <v>25</v>
       </c>
+      <c r="C14">
+        <v>2</v>
+      </c>
       <c r="D14" t="s">
         <v>22</v>
+      </c>
+      <c r="E14">
+        <v>2</v>
       </c>
     </row>
     <row r="15" spans="1:5" x14ac:dyDescent="0.3">
@@ -694,8 +724,14 @@
       <c r="B15" t="s">
         <v>19</v>
       </c>
+      <c r="C15">
+        <v>3</v>
+      </c>
       <c r="D15" t="s">
         <v>24</v>
+      </c>
+      <c r="E15">
+        <v>0</v>
       </c>
     </row>
     <row r="16" spans="1:5" x14ac:dyDescent="0.3">
@@ -705,66 +741,102 @@
       <c r="B16" t="s">
         <v>21</v>
       </c>
+      <c r="C16">
+        <v>1</v>
+      </c>
       <c r="D16" t="s">
         <v>23</v>
       </c>
-    </row>
-    <row r="17" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="E16">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="17" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A17" t="s">
         <v>3</v>
       </c>
       <c r="B17" t="s">
         <v>20</v>
       </c>
+      <c r="C17">
+        <v>2</v>
+      </c>
       <c r="D17" t="s">
         <v>26</v>
       </c>
-    </row>
-    <row r="18" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="E17">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="18" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A18" t="s">
         <v>4</v>
       </c>
       <c r="B18" t="s">
         <v>26</v>
       </c>
+      <c r="C18">
+        <v>4</v>
+      </c>
       <c r="D18" t="s">
         <v>22</v>
       </c>
-    </row>
-    <row r="19" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="E18">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="19" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A19" t="s">
         <v>4</v>
       </c>
       <c r="B19" t="s">
         <v>25</v>
       </c>
+      <c r="C19">
+        <v>1</v>
+      </c>
       <c r="D19" t="s">
         <v>19</v>
       </c>
-    </row>
-    <row r="20" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="E19">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="20" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A20" t="s">
         <v>4</v>
       </c>
       <c r="B20" t="s">
         <v>24</v>
       </c>
+      <c r="C20">
+        <v>2</v>
+      </c>
       <c r="D20" t="s">
         <v>21</v>
       </c>
-    </row>
-    <row r="21" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="E20">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="21" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A21" t="s">
         <v>4</v>
       </c>
       <c r="B21" t="s">
         <v>23</v>
       </c>
+      <c r="C21">
+        <v>2</v>
+      </c>
       <c r="D21" t="s">
         <v>20</v>
       </c>
-    </row>
-    <row r="22" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="E21">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="22" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A22" t="s">
         <v>5</v>
       </c>
@@ -775,7 +847,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="23" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="23" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A23" t="s">
         <v>5</v>
       </c>
@@ -786,7 +858,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="24" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="24" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A24" t="s">
         <v>5</v>
       </c>
@@ -797,7 +869,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="25" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="25" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A25" t="s">
         <v>5</v>
       </c>
@@ -808,7 +880,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="26" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="26" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A26" t="s">
         <v>6</v>
       </c>
@@ -819,7 +891,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="27" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="27" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A27" t="s">
         <v>6</v>
       </c>
@@ -830,7 +902,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="28" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="28" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A28" t="s">
         <v>6</v>
       </c>
@@ -841,7 +913,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="29" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="29" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A29" t="s">
         <v>6</v>
       </c>
@@ -852,7 +924,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="30" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="30" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A30" t="s">
         <v>7</v>
       </c>
@@ -863,7 +935,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="31" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="31" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A31" t="s">
         <v>7</v>
       </c>
@@ -874,7 +946,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="32" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="32" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A32" t="s">
         <v>7</v>
       </c>

</xml_diff>

<commit_message>
updated to handle empty scores
</commit_message>
<xml_diff>
--- a/scores_2.xlsx
+++ b/scores_2.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\simon\OneDrive - nd.edu\Documents\Personal_projects\WCQ_Concacaf\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AB92F7B6-0C30-47DF-AACE-02DDC4F83BA0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F8DCD266-4845-4431-823A-C88A87DE8391}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="28680" yWindow="-2115" windowWidth="20730" windowHeight="11160" xr2:uid="{26DC9B6C-8293-44D9-840D-3D50F043DF2B}"/>
   </bookViews>
@@ -468,8 +468,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B280DDF3-1ED5-4A4B-B0D8-5D25BF88B470}">
   <dimension ref="A1:E57"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A7" workbookViewId="0">
-      <selection activeCell="G20" sqref="G20"/>
+    <sheetView tabSelected="1" topLeftCell="A16" workbookViewId="0">
+      <selection activeCell="E38" sqref="E38"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -843,8 +843,14 @@
       <c r="B22" t="s">
         <v>22</v>
       </c>
+      <c r="C22">
+        <v>2</v>
+      </c>
       <c r="D22" t="s">
         <v>23</v>
+      </c>
+      <c r="E22">
+        <v>0</v>
       </c>
     </row>
     <row r="23" spans="1:5" x14ac:dyDescent="0.3">
@@ -854,8 +860,14 @@
       <c r="B23" t="s">
         <v>19</v>
       </c>
+      <c r="C23">
+        <v>2</v>
+      </c>
       <c r="D23" t="s">
         <v>26</v>
+      </c>
+      <c r="E23">
+        <v>3</v>
       </c>
     </row>
     <row r="24" spans="1:5" x14ac:dyDescent="0.3">
@@ -865,8 +877,14 @@
       <c r="B24" t="s">
         <v>21</v>
       </c>
+      <c r="C24">
+        <v>3</v>
+      </c>
       <c r="D24" t="s">
         <v>25</v>
+      </c>
+      <c r="E24">
+        <v>3</v>
       </c>
     </row>
     <row r="25" spans="1:5" x14ac:dyDescent="0.3">
@@ -876,8 +894,14 @@
       <c r="B25" t="s">
         <v>20</v>
       </c>
+      <c r="C25">
+        <v>1</v>
+      </c>
       <c r="D25" t="s">
         <v>24</v>
+      </c>
+      <c r="E25">
+        <v>2</v>
       </c>
     </row>
     <row r="26" spans="1:5" x14ac:dyDescent="0.3">
@@ -887,8 +911,14 @@
       <c r="B26" t="s">
         <v>22</v>
       </c>
+      <c r="C26">
+        <v>2</v>
+      </c>
       <c r="D26" t="s">
         <v>24</v>
+      </c>
+      <c r="E26">
+        <v>1</v>
       </c>
     </row>
     <row r="27" spans="1:5" x14ac:dyDescent="0.3">
@@ -898,8 +928,14 @@
       <c r="B27" t="s">
         <v>19</v>
       </c>
+      <c r="C27">
+        <v>1</v>
+      </c>
       <c r="D27" t="s">
         <v>23</v>
+      </c>
+      <c r="E27">
+        <v>0</v>
       </c>
     </row>
     <row r="28" spans="1:5" x14ac:dyDescent="0.3">
@@ -909,8 +945,14 @@
       <c r="B28" t="s">
         <v>21</v>
       </c>
+      <c r="C28">
+        <v>0</v>
+      </c>
       <c r="D28" t="s">
         <v>26</v>
+      </c>
+      <c r="E28">
+        <v>1</v>
       </c>
     </row>
     <row r="29" spans="1:5" x14ac:dyDescent="0.3">
@@ -920,8 +962,14 @@
       <c r="B29" t="s">
         <v>20</v>
       </c>
+      <c r="C29">
+        <v>0</v>
+      </c>
       <c r="D29" t="s">
         <v>25</v>
+      </c>
+      <c r="E29">
+        <v>0</v>
       </c>
     </row>
     <row r="30" spans="1:5" x14ac:dyDescent="0.3">
@@ -931,8 +979,14 @@
       <c r="B30" t="s">
         <v>22</v>
       </c>
+      <c r="C30">
+        <v>2</v>
+      </c>
       <c r="D30" t="s">
         <v>25</v>
+      </c>
+      <c r="E30">
+        <v>3</v>
       </c>
     </row>
     <row r="31" spans="1:5" x14ac:dyDescent="0.3">
@@ -942,8 +996,14 @@
       <c r="B31" t="s">
         <v>24</v>
       </c>
+      <c r="C31">
+        <v>1</v>
+      </c>
       <c r="D31" t="s">
         <v>19</v>
+      </c>
+      <c r="E31">
+        <v>1</v>
       </c>
     </row>
     <row r="32" spans="1:5" x14ac:dyDescent="0.3">
@@ -953,66 +1013,102 @@
       <c r="B32" t="s">
         <v>23</v>
       </c>
+      <c r="C32">
+        <v>4</v>
+      </c>
       <c r="D32" t="s">
         <v>21</v>
       </c>
-    </row>
-    <row r="33" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="E32">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="33" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A33" t="s">
         <v>7</v>
       </c>
       <c r="B33" t="s">
         <v>26</v>
       </c>
+      <c r="C33">
+        <v>1</v>
+      </c>
       <c r="D33" t="s">
         <v>20</v>
       </c>
-    </row>
-    <row r="34" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="E33">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="34" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A34" t="s">
         <v>8</v>
       </c>
       <c r="B34" t="s">
         <v>19</v>
       </c>
+      <c r="C34">
+        <v>4</v>
+      </c>
       <c r="D34" t="s">
         <v>22</v>
       </c>
-    </row>
-    <row r="35" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="E34">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="35" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A35" t="s">
         <v>8</v>
       </c>
       <c r="B35" t="s">
         <v>20</v>
       </c>
+      <c r="C35">
+        <v>0</v>
+      </c>
       <c r="D35" t="s">
         <v>21</v>
       </c>
-    </row>
-    <row r="36" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="E35">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="36" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A36" t="s">
         <v>8</v>
       </c>
       <c r="B36" t="s">
         <v>24</v>
       </c>
+      <c r="C36">
+        <v>1</v>
+      </c>
       <c r="D36" t="s">
         <v>23</v>
       </c>
-    </row>
-    <row r="37" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="E36">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="37" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A37" t="s">
         <v>8</v>
       </c>
       <c r="B37" t="s">
         <v>26</v>
       </c>
+      <c r="C37">
+        <v>2</v>
+      </c>
       <c r="D37" t="s">
         <v>25</v>
       </c>
-    </row>
-    <row r="38" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="E37">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="38" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A38" t="s">
         <v>9</v>
       </c>
@@ -1023,7 +1119,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="39" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="39" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A39" t="s">
         <v>9</v>
       </c>
@@ -1034,7 +1130,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="40" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="40" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A40" t="s">
         <v>9</v>
       </c>
@@ -1045,7 +1141,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="41" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="41" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A41" t="s">
         <v>9</v>
       </c>
@@ -1056,7 +1152,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="42" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="42" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A42" t="s">
         <v>10</v>
       </c>
@@ -1067,7 +1163,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="43" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="43" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A43" t="s">
         <v>10</v>
       </c>
@@ -1078,7 +1174,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="44" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="44" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A44" t="s">
         <v>10</v>
       </c>
@@ -1089,7 +1185,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="45" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="45" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A45" t="s">
         <v>10</v>
       </c>
@@ -1100,7 +1196,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="46" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="46" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A46" t="s">
         <v>11</v>
       </c>
@@ -1111,7 +1207,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="47" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="47" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A47" t="s">
         <v>11</v>
       </c>
@@ -1122,7 +1218,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="48" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="48" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A48" t="s">
         <v>11</v>
       </c>

</xml_diff>